<commit_message>
Refactor database migrations and seeders; add indexes, remove unused tables, and update user seeder
</commit_message>
<xml_diff>
--- a/public/file/format-import-listSto(system-sto).xlsx
+++ b/public/file/format-import-listSto(system-sto).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\system-sto-kbi\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D0BEB2-DB04-40D0-9362-09B92B236691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC75B50B-5A0B-485E-82CC-53E63FDEFC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Inv_id</t>
   </si>
@@ -31,13 +31,10 @@
     <t>part_number</t>
   </si>
   <si>
-    <t>kategori</t>
+    <t>customer</t>
   </si>
   <si>
-    <t>total_qty</t>
-  </si>
-  <si>
-    <t>customer</t>
+    <t>plan_stock</t>
   </si>
 </sst>
 </file>
@@ -153,9 +150,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -168,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -188,20 +183,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,7 +503,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,25 +527,22 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>

</xml_diff>